<commit_message>
Finished imf gdp nominal multiyear
</commit_message>
<xml_diff>
--- a/DataCleaner/DataSource/final/imf_ppp/1980.xlsx
+++ b/DataCleaner/DataSource/final/imf_ppp/1980.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,71 +446,71 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Arabic</t>
+          <t>English</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>6.637758947812254</v>
+        <v>29.3277242588475</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Bengali</t>
+          <t>Spanish</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.3754930380047538</v>
+        <v>9.798936260684197</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Chinese</t>
+          <t>Japanese</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2.981812235161721</v>
+        <v>7.953924487942714</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Dutch</t>
+          <t>German</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2.035182244778597</v>
+        <v>7.849050354031187</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>English</t>
+          <t>Arabic</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>29.3277242588475</v>
+        <v>6.637758947812254</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>French</t>
+          <t>Portuguese</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>4.616115095098641</v>
+        <v>4.790230136282012</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>German</t>
+          <t>French</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>7.849050354031187</v>
+        <v>4.616115095098641</v>
       </c>
     </row>
     <row r="9">
@@ -526,21 +526,21 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>Japanese</t>
+          <t>Chinese</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>7.953924487942714</v>
+        <v>2.981812235161721</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>Korean</t>
+          <t>Dutch</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.6158925829122258</v>
+        <v>2.035182244778597</v>
       </c>
     </row>
     <row r="12">
@@ -576,41 +576,41 @@
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>Portuguese</t>
+          <t>Turkish</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>4.790230136282012</v>
+        <v>1.185450800902381</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>Russian</t>
+          <t>Swedish</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0</v>
+        <v>0.6523747516285912</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>Spanish</t>
+          <t>Korean</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>9.798936260684197</v>
+        <v>0.6158925829122258</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>Swedish</t>
+          <t>Urdu</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.6523747516285912</v>
+        <v>0.5881381344929782</v>
       </c>
     </row>
     <row r="19">
@@ -626,40 +626,20 @@
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>Turkish</t>
+          <t>Bengali</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>1.185450800902381</v>
+        <v>0.3754930380047538</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>Urdu</t>
+          <t>Vietnamese</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.5881381344929782</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="1" t="inlineStr">
-        <is>
-          <t>Uzbek</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="1" t="inlineStr">
-        <is>
-          <t>Vietnamese</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
         <v>0.2171355532622536</v>
       </c>
     </row>

</xml_diff>